<commit_message>
Deprecate update-frequency (close #11)
</commit_message>
<xml_diff>
--- a/update-frequency/update-frequency.xlsx
+++ b/update-frequency/update-frequency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scrocca\Desktop\cefriel-github\controlled-vocabularies\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1ED5F-99E1-4187-817C-049A319EB360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7615DB38-8A33-4B63-9657-A5DC031CBFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -91,12 +91,6 @@
     <t>Update frequency</t>
   </si>
   <si>
-    <t>Up to 1min</t>
-  </si>
-  <si>
-    <t>Up to 5min</t>
-  </si>
-  <si>
     <t>Up to 10 min</t>
   </si>
   <si>
@@ -121,12 +115,6 @@
     <t>Up to 24h</t>
   </si>
   <si>
-    <t>Up to every 3month</t>
-  </si>
-  <si>
-    <t>Up to every 6month</t>
-  </si>
-  <si>
     <t>Less frequent than yearly</t>
   </si>
   <si>
@@ -190,22 +178,64 @@
     <t>Up to every 6 months</t>
   </si>
   <si>
-    <t>Extends the http://publications.europa.eu/resource/authority/frequency SKOS taxonomy.</t>
-  </si>
-  <si>
-    <t>Controlled vocabulary for the update frequency of a dataset.</t>
-  </si>
-  <si>
     <t>http://purl.org/ontology/bibo/status</t>
   </si>
   <si>
     <t>owl:priorVersion</t>
   </si>
   <si>
-    <t>Published Controlled Vocabulary</t>
-  </si>
-  <si>
     <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Deprecated Controlled Vocabulary</t>
+  </si>
+  <si>
+    <t>skos:exactMatch</t>
+  </si>
+  <si>
+    <t>owl:deprecated^^xsd:boolean</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/1MIN</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/5MIN</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/10MIN</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/15MIN</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/30MIN</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/HOURLY</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/BIHOURLY</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/TRIHOURLY</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/12HRS</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/DAILY</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/QUARTERLY</t>
+  </si>
+  <si>
+    <t>ttp://publications.europa.eu/resource/authority/frequency/ANNUAL</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/frequency/ANNUAL_2</t>
+  </si>
+  <si>
+    <t>Deprecated controlled vocabulary for the update frequency of a dataset. Terms added to the http://publications.europa.eu/resource/authority/frequency SKOS taxonomy.</t>
   </si>
 </sst>
 </file>
@@ -270,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -284,6 +314,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,7 +626,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -601,23 +634,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.42578125" customWidth="1"/>
-    <col min="2" max="2" width="74.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="55.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="105.109375" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -625,7 +659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -634,16 +668,16 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -652,7 +686,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -661,7 +695,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -670,28 +704,28 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -701,356 +735,379 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/update-frequency/1min</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f t="shared" ref="A21:A32" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B21)," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/update-frequency/5min</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B22)," ","-"),",",""))</f>
+        <v>https://w3id.org/mobilitydcat-ap/update-frequency/10min</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B19)," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/update-frequency/1min</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <f t="shared" ref="A20:A31" si="0">_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B20)," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/update-frequency/5min</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f>_xlfn.CONCAT($B$1,"/",SUBSTITUTE(SUBSTITUTE(LOWER(B21)," ","-"),",",""))</f>
-        <v>https://w3id.org/mobilitydcat-ap/update-frequency/10min</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/15min</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/30min</v>
       </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/1h</v>
       </c>
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/2h</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/3h</v>
       </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/12h</v>
       </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/24h</v>
       </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/3-months</v>
       </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/6-months</v>
       </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>https://w3id.org/mobilitydcat-ap/update-frequency/less-than-yearly</v>
       </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>30</v>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{8D37ED2A-6F4C-4B2C-B212-84B5255111B4}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{F5CCEF78-A2AE-420B-8B79-2E74A78B421A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1063,7 +1120,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>